<commit_message>
added todo list 10march20
</commit_message>
<xml_diff>
--- a/designEnFunctionaliteit.xlsx
+++ b/designEnFunctionaliteit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenten\Winc\winc-fed-projecten\kostenDeler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B75126-7CA4-45AF-AB72-69F7A3449A40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A22067-ED02-4D6F-AECB-0F11F86E3F4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{388D1EC8-615A-471C-ABFA-65060D61F4C1}"/>
+    <workbookView xWindow="-60" yWindow="135" windowWidth="23025" windowHeight="14490" xr2:uid="{388D1EC8-615A-471C-ABFA-65060D61F4C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>etentje</t>
   </si>
@@ -87,16 +87,100 @@
   </si>
   <si>
     <t>lunch</t>
+  </si>
+  <si>
+    <t>ToDo</t>
+  </si>
+  <si>
+    <t>input form maken</t>
+  </si>
+  <si>
+    <t>total amount pp maken</t>
+  </si>
+  <si>
+    <t>werkend maken:</t>
+  </si>
+  <si>
+    <t>basics:</t>
+  </si>
+  <si>
+    <t>input form werkend maken</t>
+  </si>
+  <si>
+    <t>sort buttons werkend maken</t>
+  </si>
+  <si>
+    <t>total amount pp werkend maken</t>
+  </si>
+  <si>
+    <t>extra:</t>
+  </si>
+  <si>
+    <t>communicatie met API ipv data.js</t>
+  </si>
+  <si>
+    <t>final:</t>
+  </si>
+  <si>
+    <t>hosting</t>
+  </si>
+  <si>
+    <t>delete buttons werkend maken</t>
+  </si>
+  <si>
+    <t>delete buttons toevoegen</t>
+  </si>
+  <si>
+    <t>styling</t>
+  </si>
+  <si>
+    <t>user accounts maken met inlogsysteem</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Daan</t>
+  </si>
+  <si>
+    <t>veld toevoegen en "ingevoerd door"</t>
+  </si>
+  <si>
+    <t>sort buttons wijzigen naar dropdown</t>
+  </si>
+  <si>
+    <t>Pair</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,9 +206,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -439,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703B0675-640F-479A-A5FE-AE80244B8BE5}">
-  <dimension ref="A3:N14"/>
+  <dimension ref="A3:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,10 +550,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3">
@@ -472,7 +561,8 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4">
@@ -480,7 +570,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5">
@@ -488,7 +579,8 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C6">
@@ -496,7 +588,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
@@ -514,28 +606,33 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>100</v>
       </c>
-      <c r="G11" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J11" t="s">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="3">
         <v>43893</v>
       </c>
-      <c r="M11" t="s">
+      <c r="L11" s="2"/>
+      <c r="M11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="N11" t="s">
@@ -543,25 +640,31 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>150</v>
       </c>
-      <c r="G12" t="s">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J12" t="s">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="3">
         <v>43895</v>
       </c>
-      <c r="M12" t="s">
+      <c r="L12" s="2"/>
+      <c r="M12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="N12" t="s">
@@ -569,25 +672,31 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>60</v>
       </c>
-      <c r="G13" t="s">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J13" t="s">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="3">
         <v>43896</v>
       </c>
-      <c r="M13" t="s">
+      <c r="L13" s="2"/>
+      <c r="M13" s="2" t="s">
         <v>4</v>
       </c>
       <c r="N13" t="s">
@@ -595,29 +704,147 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>50</v>
       </c>
-      <c r="G14" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J14" t="s">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="3">
         <v>43897</v>
       </c>
-      <c r="M14" t="s">
+      <c r="L14" s="2"/>
+      <c r="M14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="N14" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated ToDo's for 12 march 20
</commit_message>
<xml_diff>
--- a/designEnFunctionaliteit.xlsx
+++ b/designEnFunctionaliteit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documenten\Winc\winc-fed-projecten\kostenDeler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECD25D8-AAC5-4487-92A2-46A17B31AC46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2759B0-BC1C-47E8-9935-B357419FDED6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5910" yWindow="105" windowWidth="23025" windowHeight="14490" xr2:uid="{388D1EC8-615A-471C-ABFA-65060D61F4C1}"/>
+    <workbookView xWindow="915" yWindow="615" windowWidth="19110" windowHeight="14490" xr2:uid="{388D1EC8-615A-471C-ABFA-65060D61F4C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t>etentje</t>
   </si>
@@ -150,6 +150,48 @@
   </si>
   <si>
     <t>Pair</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>paid by</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>added by</t>
+  </si>
+  <si>
+    <t>delete item</t>
+  </si>
+  <si>
+    <t>balance fields toevoegen</t>
+  </si>
+  <si>
+    <t>balance fields werkend maken</t>
+  </si>
+  <si>
+    <t>totalAmount PP</t>
+  </si>
+  <si>
+    <t>balancePP</t>
+  </si>
+  <si>
+    <t>Meerdere groepen kunnen maken</t>
+  </si>
+  <si>
+    <t>code voor totalAmountPP DRY en KISS maken, totalAmountPP uit de .map halen</t>
   </si>
 </sst>
 </file>
@@ -174,19 +216,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF92D050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,13 +237,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -218,18 +254,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -544,17 +578,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703B0675-640F-479A-A5FE-AE80244B8BE5}">
-  <dimension ref="A3:N36"/>
+  <dimension ref="A2:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
     <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -565,225 +599,481 @@
     <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J8" t="s">
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="1"/>
-      <c r="M8" t="s">
+      <c r="K8" s="5"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S10" s="4"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="4">
         <v>100</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
+      <c r="I11" s="4"/>
+      <c r="J11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="5">
         <v>43893</v>
       </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2" t="s">
+      <c r="L11" s="4"/>
+      <c r="M11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
+      <c r="O11" s="4"/>
+      <c r="P11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="4">
         <v>150</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
+      <c r="I12" s="4"/>
+      <c r="J12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="5">
         <v>43895</v>
       </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2" t="s">
+      <c r="L12" s="4"/>
+      <c r="M12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
+      <c r="O12" s="4"/>
+      <c r="P12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="4">
         <v>60</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
+      <c r="I13" s="4"/>
+      <c r="J13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="5">
         <v>43896</v>
       </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2" t="s">
+      <c r="L13" s="4"/>
+      <c r="M13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
+      <c r="O13" s="4"/>
+      <c r="P13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="4">
         <v>50</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
+      <c r="I14" s="4"/>
+      <c r="J14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="5">
         <v>43897</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2" t="s">
+      <c r="L14" s="4"/>
+      <c r="M14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="4"/>
+      <c r="P14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="D16" s="3"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
       <c r="G19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>31</v>
       </c>
@@ -791,75 +1081,98 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="G29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>